<commit_message>
removed USDA spreadsheet because no longer used. And updated physteSources data set.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/phytateSources.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/phytateSources.xlsx
@@ -1174,7 +1174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1212,6 +1212,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1505,13 +1508,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="11"/>
+    <col min="2" max="2" width="71.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="14"/>
     <col min="5" max="5" width="10.83203125" style="6"/>
   </cols>
@@ -1538,19 +1542,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>5</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>320</v>
       </c>
       <c r="C2" s="14">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="E2" s="6">
-        <v>2128</v>
+        <v>2471</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1571,116 +1575,125 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>167</v>
+      <c r="A4" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C4" s="15">
-        <v>100</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5"/>
+        <v>221</v>
+      </c>
+      <c r="C4" s="14">
+        <v>100</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2128</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>218</v>
+      <c r="A5" s="11" t="s">
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>319</v>
       </c>
       <c r="C5" s="14">
         <v>100</v>
       </c>
+      <c r="E5" s="6">
+        <v>2128</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>219</v>
+      <c r="A6" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>308</v>
       </c>
       <c r="C6" s="14">
-        <v>100</v>
+        <v>51</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2052</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>310</v>
       </c>
       <c r="C7" s="14">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="E7" s="6">
-        <v>63</v>
+        <v>2052</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>166</v>
+      <c r="A8" s="11" t="s">
+        <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>227</v>
-      </c>
-      <c r="C8" s="15">
-        <v>100</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5"/>
+        <v>347</v>
+      </c>
+      <c r="C8" s="14">
+        <v>100</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1957</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>165</v>
+      <c r="A9" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
-      </c>
-      <c r="C9" s="15">
-        <v>100</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>345</v>
+      </c>
+      <c r="C9" s="14">
+        <v>100</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1901</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>229</v>
+        <v>307</v>
       </c>
       <c r="C10" s="14">
-        <v>93</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="E10" s="6">
-        <v>0</v>
+        <v>1728</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>6</v>
@@ -1688,36 +1701,33 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>230</v>
+        <v>344</v>
       </c>
       <c r="C11" s="14">
         <v>100</v>
       </c>
       <c r="E11" s="6">
-        <v>0</v>
+        <v>1485</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>6</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>309</v>
       </c>
       <c r="C12" s="14">
-        <v>74</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E12" s="6">
-        <v>141</v>
+        <v>1372</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>6</v>
@@ -1725,16 +1735,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>232</v>
+        <v>342</v>
       </c>
       <c r="C13" s="14">
-        <v>64</v>
+        <v>73</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E13" s="6">
-        <v>3</v>
+        <v>1314</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>6</v>
@@ -1742,39 +1755,33 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>324</v>
       </c>
       <c r="C14" s="14">
-        <v>95</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E14" s="6">
-        <v>3</v>
+        <v>1244</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s">
-        <v>234</v>
+        <v>351</v>
       </c>
       <c r="C15" s="14">
-        <v>90</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E15" s="6">
-        <v>0</v>
+        <v>1180</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>6</v>
@@ -1782,39 +1789,36 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>235</v>
+        <v>325</v>
       </c>
       <c r="C16" s="14">
-        <v>92</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E16" s="6">
-        <v>0</v>
+        <v>1041</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>236</v>
+        <v>311</v>
       </c>
       <c r="C17" s="14">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E17" s="6">
-        <v>2</v>
+        <v>943</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>6</v>
@@ -1822,172 +1826,152 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>237</v>
+        <v>353</v>
       </c>
       <c r="C18" s="14">
-        <v>98</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E18" s="6">
-        <v>2</v>
+        <v>894</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>82</v>
+      <c r="A19" s="13">
+        <v>20014</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>348</v>
       </c>
       <c r="C19" s="14">
-        <v>99</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="E19" s="6">
-        <v>30</v>
-      </c>
-      <c r="F19" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="F19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>69</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>239</v>
+        <v>349</v>
       </c>
       <c r="C20" s="14">
-        <v>96</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E20" s="6">
-        <v>101</v>
+        <v>835</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>91</v>
+      <c r="A21" s="12">
+        <v>16085</v>
       </c>
       <c r="B21" t="s">
-        <v>240</v>
+        <v>341</v>
       </c>
       <c r="C21" s="14">
         <v>100</v>
       </c>
       <c r="E21" s="6">
-        <v>7</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>6</v>
+        <v>820</v>
+      </c>
+      <c r="F21" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="B22" t="s">
-        <v>241</v>
+        <v>354</v>
       </c>
       <c r="C22" s="14">
-        <v>50</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="E22" s="6">
-        <v>0</v>
+        <v>790</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>205</v>
+      <c r="A23" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>242</v>
-      </c>
-      <c r="C23" s="15">
-        <v>100</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E23" s="4">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>340</v>
+      </c>
+      <c r="C23" s="14">
+        <v>100</v>
+      </c>
+      <c r="E23" s="6">
+        <v>770</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="B24" t="s">
-        <v>243</v>
+        <v>352</v>
       </c>
       <c r="C24" s="14">
-        <v>96</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="E24" s="6">
-        <v>7</v>
+        <v>725</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>203</v>
+      <c r="A25" s="11" t="s">
+        <v>147</v>
       </c>
       <c r="B25" t="s">
-        <v>244</v>
-      </c>
-      <c r="C25" s="15">
-        <v>100</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E25" s="4">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>346</v>
+      </c>
+      <c r="C25" s="14">
+        <v>100</v>
+      </c>
+      <c r="E25" s="6">
+        <v>697</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>245</v>
+        <v>350</v>
       </c>
       <c r="C26" s="14">
-        <v>78</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E26" s="6">
-        <v>26</v>
+        <v>682</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>6</v>
@@ -1995,39 +1979,36 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
-        <v>246</v>
+        <v>328</v>
       </c>
       <c r="C27" s="14">
-        <v>76</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E27" s="6">
-        <v>7</v>
+        <v>646</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>247</v>
+        <v>315</v>
       </c>
       <c r="C28" s="14">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="E28" s="6">
-        <v>0</v>
+        <v>620</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>6</v>
@@ -2035,28 +2016,27 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
-        <v>248</v>
-      </c>
-      <c r="C29" s="15">
-        <v>100</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E29" s="4">
-        <v>0</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>355</v>
+      </c>
+      <c r="C29" s="14">
+        <v>100</v>
+      </c>
+      <c r="E29" s="6">
+        <v>603</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>207</v>
+      <c r="A30" s="12">
+        <v>16060</v>
       </c>
       <c r="B30" t="s">
-        <v>249</v>
+        <v>337</v>
       </c>
       <c r="C30" s="15">
         <v>100</v>
@@ -2065,352 +2045,346 @@
         <v>168</v>
       </c>
       <c r="E30" s="4">
-        <v>0</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>565</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>119</v>
+      <c r="A31" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="B31" t="s">
-        <v>250</v>
+        <v>356</v>
       </c>
       <c r="C31" s="14">
-        <v>84</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E31" s="6">
-        <v>0</v>
+        <v>530</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
       <c r="B32" t="s">
-        <v>251</v>
+        <v>329</v>
       </c>
       <c r="C32" s="14">
-        <v>51</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E32" s="6">
-        <v>46</v>
+        <v>522</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>121</v>
+      <c r="A33" s="12">
+        <v>16101</v>
       </c>
       <c r="B33" t="s">
-        <v>252</v>
-      </c>
-      <c r="C33" s="14">
-        <v>80</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="6">
-        <v>0</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>6</v>
+        <v>343</v>
+      </c>
+      <c r="C33" s="15">
+        <v>100</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" s="4">
+        <v>516</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>253</v>
+        <v>330</v>
       </c>
       <c r="C34" s="14">
-        <v>73</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="E34" s="6">
-        <v>3</v>
+        <v>506</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>254</v>
-      </c>
-      <c r="C35" s="15">
-        <v>100</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>313</v>
+      </c>
+      <c r="C35" s="14">
+        <v>25</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="6">
+        <v>499</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>209</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>255</v>
-      </c>
-      <c r="C36" s="15">
-        <v>100</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" s="4">
-        <v>0</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>332</v>
+      </c>
+      <c r="C36" s="14">
+        <v>100</v>
+      </c>
+      <c r="E36" s="6">
+        <v>482</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>256</v>
+        <v>338</v>
       </c>
       <c r="C37" s="14">
-        <v>74</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="E37" s="6">
+        <v>430</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
-        <v>213</v>
-      </c>
       <c r="B38" t="s">
-        <v>257</v>
-      </c>
-      <c r="C38" s="15">
-        <v>100</v>
-      </c>
-      <c r="D38" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="C38" s="14">
+        <v>100</v>
+      </c>
+      <c r="E38" s="6">
+        <v>414</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="13">
+        <v>11215</v>
+      </c>
+      <c r="B39" t="s">
+        <v>288</v>
+      </c>
+      <c r="C39" s="14">
+        <v>87</v>
+      </c>
+      <c r="D39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="6">
+        <v>319</v>
+      </c>
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="12">
+        <v>16056</v>
+      </c>
+      <c r="B40" t="s">
+        <v>336</v>
+      </c>
+      <c r="C40" s="15">
+        <v>100</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E38" s="4">
-        <v>0</v>
-      </c>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" t="s">
-        <v>258</v>
-      </c>
-      <c r="C39" s="14">
-        <v>62</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="6">
-        <v>26</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" t="s">
-        <v>259</v>
-      </c>
-      <c r="C40" s="14">
-        <v>96</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E40" s="6">
-        <v>0</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>6</v>
+      <c r="E40" s="4">
+        <v>313</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="C41" s="14">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="E41" s="6">
-        <v>0</v>
+        <v>303</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="B42" t="s">
-        <v>261</v>
+        <v>317</v>
       </c>
       <c r="C42" s="14">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="E42" s="6">
-        <v>0</v>
+        <v>290</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>262</v>
+        <v>316</v>
       </c>
       <c r="C43" s="14">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>35</v>
+        <v>128</v>
       </c>
       <c r="E43" s="6">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
-        <v>214</v>
+      <c r="A44" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="B44" t="s">
-        <v>263</v>
-      </c>
-      <c r="C44" s="15">
-        <v>100</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E44" s="4">
-        <v>0</v>
-      </c>
-      <c r="F44" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C44" s="14">
+        <v>45</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" s="6">
+        <v>230</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>211</v>
+      <c r="A45" s="11" t="s">
+        <v>159</v>
       </c>
       <c r="B45" t="s">
-        <v>264</v>
-      </c>
-      <c r="C45" s="15">
-        <v>100</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E45" s="4">
-        <v>0</v>
-      </c>
-      <c r="F45" s="5"/>
+        <v>357</v>
+      </c>
+      <c r="C45" s="14">
+        <v>100</v>
+      </c>
+      <c r="E45" s="6">
+        <v>226</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>212</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>265</v>
-      </c>
-      <c r="C46" s="15">
-        <v>100</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E46" s="4">
-        <v>0</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>312</v>
+      </c>
+      <c r="C46" s="14">
+        <v>51</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="6">
+        <v>190</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
       <c r="C47" s="14">
-        <v>65</v>
+        <v>38</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="E47" s="6">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="C48" s="14">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E48" s="6">
-        <v>0</v>
+        <v>188</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>6</v>
@@ -2418,19 +2392,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>268</v>
+        <v>231</v>
       </c>
       <c r="C49" s="14">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="E49" s="6">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>6</v>
@@ -2438,705 +2412,706 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B50" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
       <c r="C50" s="14">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="E50" s="6">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
-        <v>270</v>
+        <v>323</v>
       </c>
       <c r="C51" s="14">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="E51" s="6">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="C52" s="14">
-        <v>96</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="E52" s="6">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="B53" t="s">
-        <v>272</v>
+        <v>314</v>
       </c>
       <c r="C53" s="14">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E53" s="6">
+        <v>88</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="13">
+        <v>11677</v>
+      </c>
+      <c r="B54" t="s">
+        <v>304</v>
+      </c>
+      <c r="C54" s="14">
+        <v>88</v>
+      </c>
+      <c r="D54" t="s">
+        <v>196</v>
+      </c>
+      <c r="E54" s="6">
+        <v>74</v>
+      </c>
+      <c r="F54" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" t="s">
+        <v>226</v>
+      </c>
+      <c r="C55" s="14">
         <v>90</v>
       </c>
-      <c r="E53" s="6">
-        <v>11</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" t="s">
-        <v>273</v>
-      </c>
-      <c r="C54" s="14">
-        <v>52</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E54" s="6">
-        <v>3</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="B55" t="s">
-        <v>274</v>
-      </c>
-      <c r="C55" s="15">
-        <v>100</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E55" s="4">
-        <v>0</v>
-      </c>
-      <c r="F55" s="5"/>
+      <c r="D55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="6">
+        <v>63</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
-        <v>57</v>
+      <c r="A56" s="13">
+        <v>11265</v>
       </c>
       <c r="B56" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="C56" s="14">
-        <v>92</v>
-      </c>
-      <c r="D56" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" t="s">
+        <v>189</v>
+      </c>
+      <c r="E56" s="6">
+        <v>63</v>
+      </c>
+      <c r="F56" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" t="s">
+        <v>279</v>
+      </c>
+      <c r="C57" s="14">
+        <v>100</v>
+      </c>
+      <c r="E57" s="6">
+        <v>60</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
+        <v>284</v>
+      </c>
+      <c r="C58" s="14">
+        <v>84</v>
+      </c>
+      <c r="E58" s="6">
         <v>58</v>
       </c>
-      <c r="E56" s="6">
-        <v>188</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="B57" t="s">
-        <v>276</v>
-      </c>
-      <c r="C57" s="15">
-        <v>100</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E57" s="4">
-        <v>0</v>
-      </c>
-      <c r="F57" s="5"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="13">
-        <v>11007</v>
-      </c>
-      <c r="B58" t="s">
-        <v>277</v>
-      </c>
-      <c r="C58" s="14">
-        <v>40</v>
-      </c>
-      <c r="D58" t="s">
-        <v>171</v>
-      </c>
-      <c r="E58" s="6">
-        <v>12.0001</v>
-      </c>
-      <c r="F58" t="s">
-        <v>172</v>
+      <c r="F58" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="13">
-        <v>11011</v>
+      <c r="A59" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="C59" s="14">
-        <v>53</v>
-      </c>
-      <c r="D59" t="s">
-        <v>173</v>
+        <v>74</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E59" s="6">
-        <v>20</v>
-      </c>
-      <c r="F59" t="s">
+        <v>50</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="11" t="s">
-        <v>75</v>
+      <c r="A60" s="13">
+        <v>11209</v>
       </c>
       <c r="B60" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="C60" s="14">
-        <v>100</v>
+        <v>81</v>
+      </c>
+      <c r="D60" t="s">
+        <v>183</v>
       </c>
       <c r="E60" s="6">
-        <v>60</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>76</v>
+        <v>49</v>
+      </c>
+      <c r="F60" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="13">
-        <v>11052</v>
+      <c r="A61" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="B61" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
       <c r="C61" s="14">
-        <v>88</v>
-      </c>
-      <c r="D61" t="s">
-        <v>174</v>
+        <v>51</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E61" s="6">
-        <v>27</v>
-      </c>
-      <c r="F61" t="s">
-        <v>175</v>
+        <v>46</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>170</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="C62" s="14">
-        <v>61</v>
-      </c>
-      <c r="D62" t="s">
-        <v>180</v>
+        <v>72</v>
       </c>
       <c r="E62" s="6">
-        <v>18</v>
-      </c>
-      <c r="F62" t="s">
-        <v>6</v>
+        <v>44</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="13">
-        <v>11109</v>
+        <v>11670</v>
       </c>
       <c r="B63" t="s">
-        <v>282</v>
+        <v>303</v>
       </c>
       <c r="C63" s="14">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D63" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E63" s="6">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="F63" t="s">
-        <v>6</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="13">
-        <v>11124</v>
+      <c r="A64" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="B64" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="C64" s="14">
-        <v>89</v>
-      </c>
-      <c r="D64" t="s">
-        <v>177</v>
+        <v>100</v>
       </c>
       <c r="E64" s="6">
-        <v>11</v>
-      </c>
-      <c r="F64" t="s">
-        <v>178</v>
+        <v>31</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>284</v>
+        <v>238</v>
       </c>
       <c r="C65" s="14">
-        <v>84</v>
+        <v>99</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="E65" s="6">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="10" t="s">
-        <v>169</v>
+      <c r="A66" s="13">
+        <v>11246</v>
       </c>
       <c r="B66" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C66" s="14">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D66" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="E66" s="6">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F66" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="13">
-        <v>11205</v>
+        <v>11052</v>
       </c>
       <c r="B67" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C67" s="14">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D67" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="E67" s="6">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F67" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="13">
-        <v>11209</v>
+      <c r="A68" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>287</v>
+        <v>245</v>
       </c>
       <c r="C68" s="14">
-        <v>81</v>
-      </c>
-      <c r="D68" t="s">
-        <v>183</v>
+        <v>78</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="E68" s="6">
-        <v>49</v>
-      </c>
-      <c r="F68" t="s">
-        <v>184</v>
+        <v>26</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="13">
-        <v>11215</v>
+      <c r="A69" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>288</v>
+        <v>258</v>
       </c>
       <c r="C69" s="14">
-        <v>87</v>
-      </c>
-      <c r="D69" t="s">
-        <v>185</v>
+        <v>62</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E69" s="6">
-        <v>319</v>
-      </c>
-      <c r="F69" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="13">
-        <v>11246</v>
+        <v>11546</v>
       </c>
       <c r="B70" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C70" s="14">
-        <v>44</v>
-      </c>
-      <c r="D70" t="s">
-        <v>186</v>
+        <v>100</v>
       </c>
       <c r="E70" s="6">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F70" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="13">
-        <v>11257</v>
+        <v>11011</v>
       </c>
       <c r="B71" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C71" s="14">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="D71" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="E71" s="6">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F71" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="13">
-        <v>11265</v>
+      <c r="A72" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="B72" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C72" s="14">
-        <v>97</v>
-      </c>
-      <c r="D72" t="s">
-        <v>189</v>
+        <v>75</v>
       </c>
       <c r="E72" s="6">
-        <v>63</v>
-      </c>
-      <c r="F72" t="s">
-        <v>190</v>
+        <v>19</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="13">
-        <v>11278</v>
+      <c r="A73" s="11" t="s">
+        <v>170</v>
       </c>
       <c r="B73" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C73" s="14">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D73" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E73" s="6">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F73" t="s">
-        <v>193</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="13">
-        <v>11282</v>
+        <v>11422</v>
       </c>
       <c r="B74" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C74" s="14">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D74" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E74" s="6">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F74" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="11" t="s">
-        <v>62</v>
+      <c r="A75" s="13">
+        <v>11007</v>
       </c>
       <c r="B75" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="C75" s="14">
-        <v>38</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
+      </c>
+      <c r="D75" t="s">
+        <v>171</v>
       </c>
       <c r="E75" s="6">
-        <v>189</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>64</v>
+        <v>12.0001</v>
+      </c>
+      <c r="F75" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="B76" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="C76" s="14">
-        <v>75</v>
+        <v>94</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E76" s="6">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="13">
-        <v>11422</v>
+        <v>11124</v>
       </c>
       <c r="B77" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="C77" s="14">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="D77" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="E77" s="6">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F77" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="13">
-        <v>11457</v>
+        <v>11278</v>
       </c>
       <c r="B78" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C78" s="14">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D78" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E78" s="6">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F78" t="s">
-        <v>6</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" t="s">
+        <v>266</v>
+      </c>
+      <c r="C79" s="14">
         <v>65</v>
       </c>
-      <c r="B79" t="s">
-        <v>298</v>
-      </c>
-      <c r="C79" s="14">
-        <v>72</v>
-      </c>
       <c r="E79" s="6">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>299</v>
+        <v>240</v>
       </c>
       <c r="C80" s="14">
         <v>100</v>
       </c>
       <c r="E80" s="6">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="13">
-        <v>11529</v>
+      <c r="A81" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>300</v>
+        <v>243</v>
       </c>
       <c r="C81" s="14">
-        <v>91</v>
-      </c>
-      <c r="D81" t="s">
-        <v>201</v>
+        <v>96</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E81" s="6">
-        <v>5</v>
-      </c>
-      <c r="F81" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="13">
-        <v>11546</v>
+      <c r="A82" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>301</v>
+        <v>246</v>
       </c>
       <c r="C82" s="14">
-        <v>100</v>
+        <v>76</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E82" s="6">
-        <v>23</v>
-      </c>
-      <c r="F82" t="s">
-        <v>202</v>
+        <v>7</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="B83" t="s">
-        <v>302</v>
+        <v>271</v>
       </c>
       <c r="C83" s="14">
-        <v>86</v>
+        <v>96</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E83" s="6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="13">
-        <v>11670</v>
+        <v>11457</v>
       </c>
       <c r="B84" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C84" s="14">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D84" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="E84" s="6">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>182</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="13">
-        <v>11677</v>
+        <v>11282</v>
       </c>
       <c r="B85" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="C85" s="14">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E85" s="6">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="F85" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="13">
-        <v>11885</v>
+        <v>11529</v>
       </c>
       <c r="B86" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C86" s="14">
-        <v>100</v>
+        <v>91</v>
+      </c>
+      <c r="D86" t="s">
+        <v>201</v>
       </c>
       <c r="E86" s="6">
         <v>5</v>
@@ -3147,73 +3122,70 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B87" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C87" s="14">
-        <v>97</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="E87" s="6">
-        <v>303</v>
+        <v>5</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="11" t="s">
-        <v>81</v>
+      <c r="A88" s="13">
+        <v>11885</v>
       </c>
       <c r="B88" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C88" s="14">
         <v>100</v>
       </c>
       <c r="E88" s="6">
-        <v>1728</v>
-      </c>
-      <c r="F88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F88" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="11" t="s">
-        <v>86</v>
+      <c r="A89" s="10" t="s">
+        <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="C89" s="14">
-        <v>51</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>87</v>
+        <v>39</v>
+      </c>
+      <c r="D89" t="s">
+        <v>179</v>
       </c>
       <c r="E89" s="6">
-        <v>2052</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>88</v>
+        <v>4</v>
+      </c>
+      <c r="F89" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>309</v>
+        <v>232</v>
       </c>
       <c r="C90" s="14">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="E90" s="6">
-        <v>1372</v>
+        <v>3</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>6</v>
@@ -3221,19 +3193,19 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B91" t="s">
+        <v>233</v>
+      </c>
+      <c r="C91" s="14">
         <v>95</v>
       </c>
-      <c r="B91" t="s">
-        <v>310</v>
-      </c>
-      <c r="C91" s="14">
-        <v>54</v>
-      </c>
       <c r="D91" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E91" s="6">
-        <v>2052</v>
+        <v>3</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>6</v>
@@ -3241,19 +3213,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="B92" t="s">
-        <v>311</v>
+        <v>253</v>
       </c>
       <c r="C92" s="14">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="E92" s="6">
-        <v>943</v>
+        <v>3</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>6</v>
@@ -3261,19 +3233,19 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="B93" t="s">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="C93" s="14">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="E93" s="6">
-        <v>190</v>
+        <v>3</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>6</v>
@@ -3281,19 +3253,19 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B94" t="s">
-        <v>313</v>
+        <v>236</v>
       </c>
       <c r="C94" s="14">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E94" s="6">
-        <v>499</v>
+        <v>2</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>6</v>
@@ -3301,186 +3273,190 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="B95" t="s">
-        <v>314</v>
+        <v>237</v>
       </c>
       <c r="C95" s="14">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="E95" s="6">
-        <v>88</v>
+        <v>2</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="11" t="s">
-        <v>125</v>
+      <c r="A96" s="13">
+        <v>11109</v>
       </c>
       <c r="B96" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C96" s="14">
-        <v>52</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>126</v>
+        <v>80</v>
+      </c>
+      <c r="D96" t="s">
+        <v>176</v>
       </c>
       <c r="E96" s="6">
-        <v>620</v>
-      </c>
-      <c r="F96" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F96" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="11" t="s">
-        <v>127</v>
+      <c r="A97" s="13">
+        <v>11205</v>
       </c>
       <c r="B97" t="s">
-        <v>316</v>
+        <v>286</v>
       </c>
       <c r="C97" s="14">
-        <v>41</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>128</v>
+        <v>97</v>
+      </c>
+      <c r="D97" t="s">
+        <v>53</v>
       </c>
       <c r="E97" s="6">
+        <v>2</v>
+      </c>
+      <c r="F97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="13">
+        <v>11257</v>
+      </c>
+      <c r="B98" t="s">
+        <v>290</v>
+      </c>
+      <c r="C98" s="14">
+        <v>80</v>
+      </c>
+      <c r="D98" t="s">
+        <v>188</v>
+      </c>
+      <c r="E98" s="6">
+        <v>2</v>
+      </c>
+      <c r="F98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B99" t="s">
+        <v>223</v>
+      </c>
+      <c r="C99" s="15">
+        <v>100</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E99" s="4">
+        <v>0</v>
+      </c>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B100" t="s">
+        <v>227</v>
+      </c>
+      <c r="C100" s="15">
+        <v>100</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E100" s="4">
+        <v>0</v>
+      </c>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B101" t="s">
+        <v>228</v>
+      </c>
+      <c r="C101" s="15">
+        <v>100</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E101" s="4">
+        <v>0</v>
+      </c>
+      <c r="F101" s="5"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" t="s">
+        <v>229</v>
+      </c>
+      <c r="C102" s="14">
+        <v>93</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" s="6">
+        <v>0</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B103" t="s">
         <v>230</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B98" t="s">
-        <v>317</v>
-      </c>
-      <c r="C98" s="14">
-        <v>53</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E98" s="6">
-        <v>290</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B99" t="s">
-        <v>318</v>
-      </c>
-      <c r="C99" s="14">
-        <v>45</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E99" s="6">
-        <v>230</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B100" t="s">
-        <v>319</v>
-      </c>
-      <c r="C100" s="14">
-        <v>100</v>
-      </c>
-      <c r="E100" s="6">
-        <v>2128</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B101" t="s">
-        <v>320</v>
-      </c>
-      <c r="C101" s="14">
-        <v>38</v>
-      </c>
-      <c r="E101" s="6">
-        <v>2471</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="8">
-        <v>14262</v>
-      </c>
-      <c r="B102" t="s">
-        <v>321</v>
-      </c>
-      <c r="C102" s="15">
-        <v>100</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E102" s="4">
+      <c r="C103" s="14">
+        <v>100</v>
+      </c>
+      <c r="E103" s="6">
         <v>0</v>
       </c>
-      <c r="F102" s="5"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="8">
-        <v>14263</v>
-      </c>
-      <c r="B103" t="s">
-        <v>322</v>
-      </c>
-      <c r="C103" s="15">
-        <v>100</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E103" s="4">
-        <v>0</v>
-      </c>
-      <c r="F103" s="5"/>
+      <c r="F103" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="B104" t="s">
-        <v>323</v>
+        <v>234</v>
       </c>
       <c r="C104" s="14">
-        <v>67</v>
+        <v>90</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="E104" s="6">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>6</v>
@@ -3488,566 +3464,594 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="B105" t="s">
-        <v>324</v>
+        <v>235</v>
       </c>
       <c r="C105" s="14">
-        <v>100</v>
+        <v>92</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="E105" s="6">
-        <v>1244</v>
+        <v>0</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="B106" t="s">
-        <v>325</v>
+        <v>241</v>
       </c>
       <c r="C106" s="14">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="E106" s="6">
-        <v>1041</v>
+        <v>0</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="11" t="s">
-        <v>160</v>
+      <c r="A107" s="8" t="s">
+        <v>205</v>
       </c>
       <c r="B107" t="s">
-        <v>326</v>
-      </c>
-      <c r="C107" s="14">
-        <v>100</v>
-      </c>
-      <c r="E107" s="3"/>
-      <c r="F107" s="2"/>
+        <v>242</v>
+      </c>
+      <c r="C107" s="15">
+        <v>100</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E107" s="4">
+        <v>0</v>
+      </c>
+      <c r="F107" s="5"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="11" t="s">
-        <v>161</v>
+      <c r="A108" s="8" t="s">
+        <v>203</v>
       </c>
       <c r="B108" t="s">
-        <v>327</v>
-      </c>
-      <c r="C108" s="14">
-        <v>100</v>
-      </c>
-      <c r="E108" s="3"/>
-      <c r="F108" s="2"/>
+        <v>244</v>
+      </c>
+      <c r="C108" s="15">
+        <v>100</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E108" s="4">
+        <v>0</v>
+      </c>
+      <c r="F108" s="5"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="B109" t="s">
-        <v>328</v>
+        <v>247</v>
       </c>
       <c r="C109" s="14">
-        <v>100</v>
+        <v>53</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="E109" s="6">
-        <v>646</v>
+        <v>0</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>138</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>139</v>
+        <v>206</v>
       </c>
       <c r="B110" t="s">
-        <v>329</v>
-      </c>
-      <c r="C110" s="14">
-        <v>100</v>
-      </c>
-      <c r="E110" s="6">
-        <v>522</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>140</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="C110" s="15">
+        <v>100</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E110" s="4">
+        <v>0</v>
+      </c>
+      <c r="F110" s="5"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="11" t="s">
-        <v>43</v>
+      <c r="A111" s="8" t="s">
+        <v>207</v>
       </c>
       <c r="B111" t="s">
-        <v>330</v>
-      </c>
-      <c r="C111" s="14">
-        <v>100</v>
-      </c>
-      <c r="E111" s="6">
-        <v>506</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="C111" s="15">
+        <v>100</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E111" s="4">
+        <v>0</v>
+      </c>
+      <c r="F111" s="5"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>162</v>
+        <v>119</v>
       </c>
       <c r="B112" t="s">
-        <v>331</v>
+        <v>250</v>
       </c>
       <c r="C112" s="14">
-        <v>100</v>
-      </c>
-      <c r="E112" s="3"/>
-      <c r="F112" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E112" s="6">
+        <v>0</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="B113" t="s">
-        <v>332</v>
+        <v>252</v>
       </c>
       <c r="C113" s="14">
-        <v>100</v>
+        <v>80</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="E113" s="6">
-        <v>482</v>
+        <v>0</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>142</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
       <c r="B114" t="s">
-        <v>333</v>
-      </c>
-      <c r="C114" s="14">
-        <v>100</v>
-      </c>
-      <c r="E114" s="3"/>
-      <c r="F114" s="2"/>
+        <v>254</v>
+      </c>
+      <c r="C114" s="15">
+        <v>100</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E114" s="4">
+        <v>0</v>
+      </c>
+      <c r="F114" s="5"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
       <c r="B115" t="s">
-        <v>334</v>
-      </c>
-      <c r="C115" s="14">
-        <v>100</v>
-      </c>
-      <c r="E115" s="3"/>
-      <c r="F115" s="2"/>
+        <v>255</v>
+      </c>
+      <c r="C115" s="15">
+        <v>100</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E115" s="4">
+        <v>0</v>
+      </c>
+      <c r="F115" s="5"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116" s="18">
-        <v>16055</v>
+      <c r="A116" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="B116" t="s">
-        <v>335</v>
-      </c>
-      <c r="C116" s="14">
-        <v>100</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="C116" s="15">
+        <v>100</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E116" s="4">
+        <v>0</v>
+      </c>
+      <c r="F116" s="5"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="12">
-        <v>16056</v>
+      <c r="A117" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="B117" t="s">
-        <v>336</v>
-      </c>
-      <c r="C117" s="15">
-        <v>100</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E117" s="4">
-        <v>313</v>
-      </c>
-      <c r="F117" s="5" t="s">
-        <v>215</v>
+        <v>259</v>
+      </c>
+      <c r="C117" s="14">
+        <v>96</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E117" s="6">
+        <v>0</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="12">
-        <v>16060</v>
+      <c r="A118" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="B118" t="s">
-        <v>337</v>
-      </c>
-      <c r="C118" s="15">
-        <v>100</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E118" s="4">
-        <v>565</v>
-      </c>
-      <c r="F118" s="5" t="s">
-        <v>216</v>
+        <v>260</v>
+      </c>
+      <c r="C118" s="14">
+        <v>90</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E118" s="6">
+        <v>0</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B119" t="s">
-        <v>338</v>
+        <v>261</v>
       </c>
       <c r="C119" s="14">
-        <v>100</v>
+        <v>82</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="E119" s="6">
-        <v>430</v>
+        <v>0</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B120" t="s">
-        <v>339</v>
+        <v>262</v>
       </c>
       <c r="C120" s="14">
-        <v>100</v>
+        <v>51</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E120" s="6">
-        <v>414</v>
+        <v>0</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="11" t="s">
-        <v>32</v>
+      <c r="A121" s="8" t="s">
+        <v>214</v>
       </c>
       <c r="B121" t="s">
-        <v>340</v>
-      </c>
-      <c r="C121" s="14">
-        <v>100</v>
-      </c>
-      <c r="E121" s="6">
-        <v>770</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>33</v>
+        <v>263</v>
+      </c>
+      <c r="C121" s="15">
+        <v>100</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E121" s="4">
+        <v>0</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" s="12">
-        <v>16085</v>
+      <c r="A122" s="8" t="s">
+        <v>211</v>
       </c>
       <c r="B122" t="s">
-        <v>341</v>
-      </c>
-      <c r="C122" s="14">
-        <v>100</v>
-      </c>
-      <c r="E122" s="6">
-        <v>820</v>
-      </c>
-      <c r="F122" t="s">
-        <v>198</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="C122" s="15">
+        <v>100</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E122" s="4">
+        <v>0</v>
+      </c>
+      <c r="F122" s="5"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
-        <v>19</v>
+        <v>212</v>
       </c>
       <c r="B123" t="s">
-        <v>342</v>
-      </c>
-      <c r="C123" s="14">
-        <v>73</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E123" s="6">
-        <v>1314</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="C123" s="15">
+        <v>100</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E123" s="4">
+        <v>0</v>
+      </c>
+      <c r="F123" s="5"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" s="12">
-        <v>16101</v>
+      <c r="A124" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="B124" t="s">
-        <v>343</v>
-      </c>
-      <c r="C124" s="15">
-        <v>100</v>
-      </c>
-      <c r="D124" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E124" s="4">
-        <v>516</v>
-      </c>
-      <c r="F124" s="5" t="s">
-        <v>217</v>
+        <v>267</v>
+      </c>
+      <c r="C124" s="14">
+        <v>94</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E124" s="6">
+        <v>0</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="B125" t="s">
-        <v>344</v>
+        <v>268</v>
       </c>
       <c r="C125" s="14">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E125" s="6">
-        <v>1485</v>
+        <v>0</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>145</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
-        <v>146</v>
+        <v>41</v>
       </c>
       <c r="B126" t="s">
-        <v>345</v>
+        <v>269</v>
       </c>
       <c r="C126" s="14">
-        <v>100</v>
+        <v>61</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E126" s="6">
-        <v>1901</v>
+        <v>0</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127" s="11" t="s">
-        <v>147</v>
+      <c r="A127" s="8" t="s">
+        <v>204</v>
       </c>
       <c r="B127" t="s">
-        <v>346</v>
-      </c>
-      <c r="C127" s="14">
-        <v>100</v>
-      </c>
-      <c r="E127" s="6">
-        <v>697</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="C127" s="15">
+        <v>100</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E127" s="4">
+        <v>0</v>
+      </c>
+      <c r="F127" s="5"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" s="11" t="s">
-        <v>148</v>
+      <c r="A128" s="8" t="s">
+        <v>208</v>
       </c>
       <c r="B128" t="s">
-        <v>347</v>
-      </c>
-      <c r="C128" s="14">
-        <v>100</v>
-      </c>
-      <c r="E128" s="6">
-        <v>1957</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="C128" s="15">
+        <v>100</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E128" s="4">
+        <v>0</v>
+      </c>
+      <c r="F128" s="5"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" s="13">
-        <v>20014</v>
+      <c r="A129" s="8">
+        <v>14262</v>
       </c>
       <c r="B129" t="s">
-        <v>348</v>
-      </c>
-      <c r="C129" s="14">
-        <v>100</v>
-      </c>
-      <c r="E129" s="6">
-        <v>835</v>
-      </c>
-      <c r="F129" t="s">
-        <v>6</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="C129" s="15">
+        <v>100</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E129" s="4">
+        <v>0</v>
+      </c>
+      <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130" s="11" t="s">
-        <v>149</v>
+      <c r="A130" s="8">
+        <v>14263</v>
       </c>
       <c r="B130" t="s">
-        <v>349</v>
-      </c>
-      <c r="C130" s="14">
-        <v>77</v>
-      </c>
-      <c r="E130" s="6">
-        <v>835</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="C130" s="15">
+        <v>100</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E130" s="4">
+        <v>0</v>
+      </c>
+      <c r="F130" s="5"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131" s="11" t="s">
-        <v>150</v>
+      <c r="A131" s="7" t="s">
+        <v>218</v>
       </c>
       <c r="B131" t="s">
-        <v>350</v>
+        <v>224</v>
       </c>
       <c r="C131" s="14">
         <v>100</v>
       </c>
-      <c r="E131" s="6">
-        <v>682</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132" s="11" t="s">
-        <v>151</v>
+      <c r="A132" s="7" t="s">
+        <v>219</v>
       </c>
       <c r="B132" t="s">
-        <v>351</v>
+        <v>225</v>
       </c>
       <c r="C132" s="14">
         <v>100</v>
-      </c>
-      <c r="E132" s="6">
-        <v>1180</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B133" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="C133" s="14">
         <v>100</v>
       </c>
-      <c r="E133" s="6">
-        <v>725</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E133" s="3"/>
+      <c r="F133" s="2"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B134" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="C134" s="14">
         <v>100</v>
       </c>
-      <c r="E134" s="6">
-        <v>894</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E134" s="3"/>
+      <c r="F134" s="2"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B135" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="C135" s="14">
         <v>100</v>
       </c>
-      <c r="E135" s="6">
-        <v>790</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>155</v>
-      </c>
+      <c r="E135" s="3"/>
+      <c r="F135" s="2"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B136" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="C136" s="14">
         <v>100</v>
       </c>
-      <c r="E136" s="6">
-        <v>603</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E136" s="3"/>
+      <c r="F136" s="2"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="16" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B137" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="C137" s="14">
         <v>100</v>
       </c>
-      <c r="E137" s="6">
-        <v>530</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="E137" s="3"/>
+      <c r="F137" s="2"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A138" s="11" t="s">
-        <v>159</v>
+      <c r="A138" s="18">
+        <v>16055</v>
       </c>
       <c r="B138" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="C138" s="14">
         <v>100</v>
-      </c>
-      <c r="E138" s="6">
-        <v>226</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -4083,8 +4087,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F61">
-    <sortState ref="A2:E116">
-      <sortCondition ref="A1:A116"/>
+    <sortState ref="A2:F138">
+      <sortCondition descending="1" ref="E1:E138"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:E209">

</xml_diff>